<commit_message>
Tests complete with final tweaks with README.md updated.
</commit_message>
<xml_diff>
--- a/src/resources/data/testData.xlsx
+++ b/src/resources/data/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tshan\OneDrive\Desktop\AMPOL\playwright-challenge\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CE2B7B-C38B-467B-B3BD-3E43D072D37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03703C7E-A73A-4CF2-9E6F-47CA35543242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>TestName</t>
   </si>
@@ -42,14 +42,20 @@
     <t>YES</t>
   </si>
   <si>
-    <t>RESTUserTest</t>
+    <t>parallel</t>
+  </si>
+  <si>
+    <t>WeatherRESTAPITest</t>
+  </si>
+  <si>
+    <t>EnergyUITest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +70,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,9 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,14 +409,25 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>